<commit_message>
Fixed Spelling errors in Revision table
</commit_message>
<xml_diff>
--- a/Docs/Sprint Revisions.xlsx
+++ b/Docs/Sprint Revisions.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephen\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephen\Documents\NetBeansProjects\Team-1-CMSC-495\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
   <si>
     <t>Group 1 - Revision Table</t>
   </si>
@@ -47,9 +47,6 @@
     <t>Create Initial Data File</t>
   </si>
   <si>
-    <t>Created Data File and added URL and Decription for each Lift/WOD</t>
-  </si>
-  <si>
     <t>Stephen</t>
   </si>
   <si>
@@ -80,9 +77,6 @@
     <t>Modified GUIs</t>
   </si>
   <si>
-    <t>Modified GUIs and sucessfully linked data.  Made graphical enhancements.</t>
-  </si>
-  <si>
     <t>Created Lift and WOD Objects</t>
   </si>
   <si>
@@ -101,30 +95,15 @@
     <t>To and From Data File</t>
   </si>
   <si>
-    <t>Completed the To and From Datafile Methods</t>
-  </si>
-  <si>
     <t>Completed GUI Modifications</t>
   </si>
   <si>
-    <t>Standardized the GUIs to give them a uniform and more professionsal look.  Also, changed the buttons</t>
-  </si>
-  <si>
     <t>Completed the Backup Data File</t>
   </si>
   <si>
     <t>Completed the Backup Data File to ensure that if the primary data file is corrupted it can be read from the last known-good backup</t>
   </si>
   <si>
-    <t>Stepehn</t>
-  </si>
-  <si>
-    <t>Tanksgiving</t>
-  </si>
-  <si>
-    <t>Sent group a toutorial on using GitHub with NetBeans</t>
-  </si>
-  <si>
     <t>Error Handling</t>
   </si>
   <si>
@@ -141,6 +120,24 @@
   </si>
   <si>
     <t>Added method to update Backup Data File upon successful read from primary data file</t>
+  </si>
+  <si>
+    <t>Created Data File and added URL and Description for each Lift/WOD</t>
+  </si>
+  <si>
+    <t>Modified GUIs and successfully linked data.  Made graphical enhancements.</t>
+  </si>
+  <si>
+    <t>Completed the To and From Data file Methods</t>
+  </si>
+  <si>
+    <t>Standardized the GUIs to give them a uniform and more professional look.  Also, changed the buttons</t>
+  </si>
+  <si>
+    <t>Thanksgiving</t>
+  </si>
+  <si>
+    <t>Sent group a tutorial on using GitHub with NetBeans</t>
   </si>
 </sst>
 </file>
@@ -218,9 +215,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -242,6 +236,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -526,7 +523,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="A1:D17"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -538,229 +535,229 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="8" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
+      <c r="A4" s="4">
         <v>41966</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="3" t="s">
+    </row>
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>41967</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
+      <c r="D5" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
         <v>41967</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>41968</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
-        <v>41967</v>
-      </c>
-      <c r="B6" s="4" t="s">
+    </row>
+    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>41968</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>41968</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
-        <v>41968</v>
-      </c>
-      <c r="B7" s="4" t="s">
+    </row>
+    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>41969</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>41969</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>41969</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>41970</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>41971</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>41971</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C15" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
-        <v>41968</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
-        <v>41968</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
-        <v>41969</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
-        <v>41969</v>
-      </c>
-      <c r="B11" s="4" t="s">
+      <c r="D15" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
+        <v>41972</v>
+      </c>
+      <c r="B16" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C16" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="90" x14ac:dyDescent="0.25">
-      <c r="A12" s="5">
-        <v>41969</v>
-      </c>
-      <c r="B12" s="4" t="s">
+      <c r="D16" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
+        <v>41972</v>
+      </c>
+      <c r="B17" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C17" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="5">
-        <v>41970</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
-        <v>41971</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="5">
-        <v>41971</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="6">
-        <v>41972</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="6">
-        <v>41972</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>13</v>
+      <c r="D17" s="7" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>